<commit_message>
Update test cases excel
</commit_message>
<xml_diff>
--- a/test-data/test_cases.xlsx
+++ b/test-data/test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\playwright-ddt-framework\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02D0D1B-B2E8-4785-B1F9-D2A3C48FAE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99125DC-6D99-42CC-BC4E-4209FC3EFE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9930" yWindow="10690" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{4B3D6F45-7A48-4EC2-909B-72731C307B29}"/>
   </bookViews>
@@ -90,9 +90,6 @@
     <t>parkingLot</t>
   </si>
   <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>08/24/2025</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>Valet Parking - Exit Before Entry</t>
+  </si>
+  <si>
+    <t>expectedError</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +618,7 @@
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -633,7 +633,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -644,16 +644,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>